<commit_message>
1:20am grind session, I hate you pk for sleeping
</commit_message>
<xml_diff>
--- a/backend/public/formatted_output.xlsx
+++ b/backend/public/formatted_output.xlsx
@@ -1082,7 +1082,7 @@
     <t>PO Attainment Table</t>
   </si>
   <si>
-    <t>CO Attainment in %</t>
+    <t>CO Attainment</t>
   </si>
   <si>
     <t>CO RESULT</t>
@@ -10606,7 +10606,7 @@
         <v>3.5999999999999996</v>
       </c>
       <c r="I156" s="40">
-        <v>7.199999999999999</v>
+        <v>10.799999999999999</v>
       </c>
       <c r="J156" s="40">
         <v>3.5999999999999996</v>
@@ -10661,7 +10661,7 @@
         <v>138</v>
       </c>
       <c r="I157" s="40">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J157" s="40">
         <v>136</v>
@@ -10771,7 +10771,7 @@
         <v>100</v>
       </c>
       <c r="I159" s="40">
-        <v>99.27</v>
+        <v>97.81</v>
       </c>
       <c r="J159" s="40">
         <v>100</v>
@@ -11020,13 +11020,13 @@
         <v>22</v>
       </c>
       <c r="B166" s="40">
-        <v>98.07</v>
+        <v>97.34</v>
       </c>
       <c r="C166" s="40">
         <v>63.5</v>
       </c>
       <c r="D166" s="40">
-        <v>80.78</v>
+        <v>80.42</v>
       </c>
       <c r="E166" s="40">
         <v>3</v>
@@ -11052,7 +11052,7 @@
         <v>311</v>
       </c>
       <c r="N166" s="40">
-        <v>99.27</v>
+        <v>97.81</v>
       </c>
       <c r="O166" s="40">
         <v>96.88</v>
@@ -11064,7 +11064,7 @@
         <v>311</v>
       </c>
       <c r="R166" s="40">
-        <v>98.07</v>
+        <v>97.34</v>
       </c>
     </row>
     <row r="167" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>